<commit_message>
update mum, C, recruit kdenr
</commit_message>
<xml_diff>
--- a/R/Init_nums_scalar_for_recruits.xlsx
+++ b/R/Init_nums_scalar_for_recruits.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20250" windowHeight="9930" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20250" windowHeight="9930" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="vert_order" sheetId="3" r:id="rId1"/>
@@ -19,14 +19,15 @@
     <sheet name="20190301" sheetId="6" r:id="rId5"/>
     <sheet name="20190422" sheetId="7" r:id="rId6"/>
     <sheet name="20190507" sheetId="8" r:id="rId7"/>
-    <sheet name="codenames" sheetId="2" r:id="rId8"/>
+    <sheet name="20190513" sheetId="9" r:id="rId8"/>
+    <sheet name="codenames" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2268" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2448" uniqueCount="450">
   <si>
     <t>species</t>
   </si>
@@ -1373,6 +1374,9 @@
   </si>
   <si>
     <t>To USE 20190228</t>
+  </si>
+  <si>
+    <t>TO USE: SELECT ALL, SORT ON COLUMN 'D', PASTE ALPHBETICALLY SORTED RECRTUIT SCALAR; SORT COL 'A'; PASTE RECRUIT KDENR_XXX FROM BIOL FILE INTO COL 'G'; COPY AND PASTE VALS FROM 'J'</t>
   </si>
 </sst>
 </file>
@@ -24580,8 +24584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M178"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28385,6 +28389,3820 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M179"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>INDEX($G:G,A2)</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>0.96637251733206997</v>
+      </c>
+      <c r="G3" s="2">
+        <v>8555604</v>
+      </c>
+      <c r="J3" t="e">
+        <f>INDEX($G:$G,A3)*(INDEX($E:$E,A3))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L3" s="2">
+        <v>8267900.5747763272</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <f>INDEX($G:$G,A4)</f>
+        <v>8555604</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <f>INDEX($G:G,A5)</f>
+        <v>0</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>4.4628380472135403</v>
+      </c>
+      <c r="G6" s="2">
+        <v>214406308</v>
+      </c>
+      <c r="J6" t="e">
+        <f>INDEX($G:$G,A6)*(INDEX($E:$E,A6))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L6" s="2">
+        <v>956860628.90498483</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f>INDEX($G:$G,A7)</f>
+        <v>214406308</v>
+      </c>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f>INDEX($G:G,A8)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9">
+        <v>0.95920413992228204</v>
+      </c>
+      <c r="G9" s="2">
+        <v>56487630</v>
+      </c>
+      <c r="J9" t="e">
+        <f>INDEX($G:$G,A9)*(INDEX($E:$E,A9))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L9" s="2">
+        <v>54183168.550398096</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <f>INDEX($G:$G,A10)</f>
+        <v>56487630</v>
+      </c>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <f>INDEX($G:G,A11)</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12">
+        <v>0.98031000543831803</v>
+      </c>
+      <c r="G12" s="2">
+        <v>530748</v>
+      </c>
+      <c r="J12" t="e">
+        <f>INDEX($G:$G,A12)*(INDEX($E:$E,A12))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L12" s="2">
+        <v>520297.57476637641</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <f>INDEX($G:$G,A13)</f>
+        <v>530748</v>
+      </c>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <f>INDEX($G:G,A14)</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15">
+        <v>0.81838242346125001</v>
+      </c>
+      <c r="G15" s="2">
+        <v>8108077</v>
+      </c>
+      <c r="J15" t="e">
+        <f>INDEX($G:$G,A15)*(INDEX($E:$E,A15))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L15" s="2">
+        <v>6635507.7048704214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="J16">
+        <f>INDEX($G:$G,A16)</f>
+        <v>8108077</v>
+      </c>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f>INDEX($G:G,A17)</f>
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18">
+        <v>2.5126606057937799</v>
+      </c>
+      <c r="G18" s="2">
+        <v>646358</v>
+      </c>
+      <c r="J18" t="e">
+        <f>INDEX($G:$G,A18)*(INDEX($E:$E,A18))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1624078.283839656</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <f>INDEX($G:$G,A19)</f>
+        <v>646358</v>
+      </c>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>6</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <f>INDEX($G:G,A20)</f>
+        <v>0</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21">
+        <v>0.72083764035817899</v>
+      </c>
+      <c r="G21" s="2">
+        <v>5349942</v>
+      </c>
+      <c r="J21" t="e">
+        <f>INDEX($G:$G,A21)*(INDEX($E:$E,A21))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L21" s="2">
+        <v>3856439.5673331167</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="J22">
+        <f>INDEX($G:$G,A22)</f>
+        <v>5349942</v>
+      </c>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <f>INDEX($G:G,A23)</f>
+        <v>0</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24">
+        <v>0.786269369075005</v>
+      </c>
+      <c r="G24" s="2">
+        <v>11650218</v>
+      </c>
+      <c r="J24" t="e">
+        <f>INDEX($G:$G,A24)*(INDEX($E:$E,A24))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L24" s="2">
+        <v>9160209.5564462673</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="J25">
+        <f>INDEX($G:$G,A25)</f>
+        <v>11650218</v>
+      </c>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <f>INDEX($G:G,A26)</f>
+        <v>0</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+      <c r="E27">
+        <v>0.55194389416626599</v>
+      </c>
+      <c r="G27" s="2">
+        <v>28167</v>
+      </c>
+      <c r="J27" t="e">
+        <f>INDEX($G:$G,A27)*(INDEX($E:$E,A27))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L27" s="2">
+        <v>15546.603666981215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="J28">
+        <f>INDEX($G:$G,A28)</f>
+        <v>28167</v>
+      </c>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <f>INDEX($G:G,A29)</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>0.670791676503252</v>
+      </c>
+      <c r="G30" s="2">
+        <v>15579871</v>
+      </c>
+      <c r="J30" t="e">
+        <f>INDEX($G:$G,A30)*(INDEX($E:$E,A30))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L30" s="2">
+        <v>10450847.787794398</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="J31">
+        <f>INDEX($G:$G,A31)</f>
+        <v>15579871</v>
+      </c>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <f>INDEX($G:G,A32)</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>11</v>
+      </c>
+      <c r="C33">
+        <v>11</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33">
+        <v>0.81964309327406004</v>
+      </c>
+      <c r="G33" s="2">
+        <v>8314004</v>
+      </c>
+      <c r="J33" t="e">
+        <f>INDEX($G:$G,A33)*(INDEX($E:$E,A33))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L33" s="2">
+        <v>6814515.9560529087</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>11</v>
+      </c>
+      <c r="J34">
+        <f>INDEX($G:$G,A34)</f>
+        <v>8314004</v>
+      </c>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>11</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="J35">
+        <f>INDEX($G:G,A35)</f>
+        <v>0</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>70</v>
+      </c>
+      <c r="E36">
+        <v>0.962307478281057</v>
+      </c>
+      <c r="G36" s="2">
+        <v>996792</v>
+      </c>
+      <c r="J36" t="e">
+        <f>INDEX($G:$G,A36)*(INDEX($E:$E,A36))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L36" s="2">
+        <v>959220.39589073136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="J37">
+        <f>INDEX($G:$G,A37)</f>
+        <v>996792</v>
+      </c>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>12</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="J38">
+        <f>INDEX($G:G,A38)</f>
+        <v>0</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="M38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>13</v>
+      </c>
+      <c r="C39">
+        <v>13</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <v>2.0896744378886201</v>
+      </c>
+      <c r="G39" s="2">
+        <v>2285</v>
+      </c>
+      <c r="J39" t="e">
+        <f>INDEX($G:$G,A39)*(INDEX($E:$E,A39))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L39" s="2">
+        <v>4774.9060905754968</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>13</v>
+      </c>
+      <c r="J40">
+        <f>INDEX($G:$G,A40)</f>
+        <v>2285</v>
+      </c>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>13</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="J41">
+        <f>INDEX($G:G,A41)</f>
+        <v>0</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>14</v>
+      </c>
+      <c r="C42">
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42">
+        <v>2.0897310451316899</v>
+      </c>
+      <c r="G42" s="2">
+        <v>31252</v>
+      </c>
+      <c r="J42" t="e">
+        <f>INDEX($G:$G,A42)*(INDEX($E:$E,A42))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L42" s="2">
+        <v>65308.274622455574</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>14</v>
+      </c>
+      <c r="J43">
+        <f>INDEX($G:$G,A43)</f>
+        <v>31252</v>
+      </c>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>14</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="J44">
+        <f>INDEX($G:G,A44)</f>
+        <v>0</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>15</v>
+      </c>
+      <c r="C45">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E45">
+        <v>2.0897139078652498</v>
+      </c>
+      <c r="G45" s="2">
+        <v>1326</v>
+      </c>
+      <c r="J45" t="e">
+        <f>INDEX($G:$G,A45)*(INDEX($E:$E,A45))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L45" s="2">
+        <v>2770.960641829321</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>15</v>
+      </c>
+      <c r="J46">
+        <f>INDEX($G:$G,A46)</f>
+        <v>1326</v>
+      </c>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>15</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <f>INDEX($G:G,A47)</f>
+        <v>0</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>16</v>
+      </c>
+      <c r="C48">
+        <v>16</v>
+      </c>
+      <c r="D48" t="s">
+        <v>54</v>
+      </c>
+      <c r="E48">
+        <v>0.95804837171452195</v>
+      </c>
+      <c r="G48" s="2">
+        <v>786817</v>
+      </c>
+      <c r="J48" t="e">
+        <f>INDEX($G:$G,A48)*(INDEX($E:$E,A48))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L48" s="2">
+        <v>753808.745687305</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>16</v>
+      </c>
+      <c r="J49">
+        <f>INDEX($G:$G,A49)</f>
+        <v>786817</v>
+      </c>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>16</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="J50">
+        <f>INDEX($G:G,A50)</f>
+        <v>0</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>17</v>
+      </c>
+      <c r="C51">
+        <v>17</v>
+      </c>
+      <c r="D51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E51">
+        <v>0.97789950966908001</v>
+      </c>
+      <c r="G51" s="2">
+        <v>20126625</v>
+      </c>
+      <c r="J51" t="e">
+        <f>INDEX($G:$G,A51)*(INDEX($E:$E,A51))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L51" s="2">
+        <v>19681816.718793448</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>17</v>
+      </c>
+      <c r="J52">
+        <f>INDEX($G:$G,A52)</f>
+        <v>20126625</v>
+      </c>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>17</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="J53">
+        <f>INDEX($G:G,A53)</f>
+        <v>0</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>18</v>
+      </c>
+      <c r="C54">
+        <v>18</v>
+      </c>
+      <c r="D54" t="s">
+        <v>12</v>
+      </c>
+      <c r="E54">
+        <v>0.99028932464642905</v>
+      </c>
+      <c r="G54" s="2">
+        <v>114125378</v>
+      </c>
+      <c r="J54" t="e">
+        <f>INDEX($G:$G,A54)*(INDEX($E:$E,A54))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L54" s="2">
+        <v>113017143.50463843</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>18</v>
+      </c>
+      <c r="J55">
+        <f>INDEX($G:$G,A55)</f>
+        <v>114125378</v>
+      </c>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>18</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <f>INDEX($G:G,A56)</f>
+        <v>0</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="M56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>19</v>
+      </c>
+      <c r="C57">
+        <v>19</v>
+      </c>
+      <c r="D57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E57">
+        <v>0.986622337721765</v>
+      </c>
+      <c r="G57" s="2">
+        <v>29144047</v>
+      </c>
+      <c r="J57" t="e">
+        <f>INDEX($G:$G,A57)*(INDEX($E:$E,A57))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L57" s="2">
+        <v>28754167.781812992</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>19</v>
+      </c>
+      <c r="J58">
+        <f>INDEX($G:$G,A58)</f>
+        <v>29144047</v>
+      </c>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>19</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="J59">
+        <f>INDEX($G:G,A59)</f>
+        <v>0</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="M59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>20</v>
+      </c>
+      <c r="C60">
+        <v>20</v>
+      </c>
+      <c r="D60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60">
+        <v>5.8671820799648504</v>
+      </c>
+      <c r="G60" s="2">
+        <v>100277557</v>
+      </c>
+      <c r="J60" t="e">
+        <f>INDEX($G:$G,A60)*(INDEX($E:$E,A60))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L60" s="2">
+        <v>588346685.45305383</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>20</v>
+      </c>
+      <c r="J61">
+        <f>INDEX($G:$G,A61)</f>
+        <v>100277557</v>
+      </c>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>20</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="H62">
+        <v>1</v>
+      </c>
+      <c r="J62">
+        <f>INDEX($G:G,A62)</f>
+        <v>0</v>
+      </c>
+      <c r="L62" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="M62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>21</v>
+      </c>
+      <c r="C63">
+        <v>21</v>
+      </c>
+      <c r="D63" t="s">
+        <v>22</v>
+      </c>
+      <c r="E63">
+        <v>0.96637768312420003</v>
+      </c>
+      <c r="G63" s="2">
+        <v>24288764</v>
+      </c>
+      <c r="J63" t="e">
+        <f>INDEX($G:$G,A63)*(INDEX($E:$E,A63))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L63" s="2">
+        <v>23472119.480270479</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>21</v>
+      </c>
+      <c r="J64">
+        <f>INDEX($G:$G,A64)</f>
+        <v>24288764</v>
+      </c>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>21</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="J65">
+        <f>INDEX($G:G,A65)</f>
+        <v>0</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="M65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>22</v>
+      </c>
+      <c r="C66">
+        <v>22</v>
+      </c>
+      <c r="D66" t="s">
+        <v>92</v>
+      </c>
+      <c r="E66">
+        <v>0.97968872431844101</v>
+      </c>
+      <c r="G66" s="2">
+        <v>3123761</v>
+      </c>
+      <c r="J66" t="e">
+        <f>INDEX($G:$G,A66)*(INDEX($E:$E,A66))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L66" s="2">
+        <v>3060313.4291656977</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>22</v>
+      </c>
+      <c r="J67">
+        <f>INDEX($G:$G,A67)</f>
+        <v>3123761</v>
+      </c>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>22</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="H68">
+        <v>1</v>
+      </c>
+      <c r="J68">
+        <f>INDEX($G:G,A68)</f>
+        <v>0</v>
+      </c>
+      <c r="L68" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>23</v>
+      </c>
+      <c r="C69">
+        <v>23</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69">
+        <v>0.98175998648196605</v>
+      </c>
+      <c r="G69" s="2">
+        <v>7461552</v>
+      </c>
+      <c r="J69" t="e">
+        <f>INDEX($G:$G,A69)*(INDEX($E:$E,A69))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L69" s="2">
+        <v>7325453.1906544864</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>23</v>
+      </c>
+      <c r="J70">
+        <f>INDEX($G:$G,A70)</f>
+        <v>7461552</v>
+      </c>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>23</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+      <c r="J71">
+        <f>INDEX($G:G,A71)</f>
+        <v>0</v>
+      </c>
+      <c r="L71" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>24</v>
+      </c>
+      <c r="C72">
+        <v>24</v>
+      </c>
+      <c r="D72" t="s">
+        <v>94</v>
+      </c>
+      <c r="E72">
+        <v>0.96602562986824603</v>
+      </c>
+      <c r="G72" s="2">
+        <v>375827441</v>
+      </c>
+      <c r="J72" t="e">
+        <f>INDEX($G:$G,A72)*(INDEX($E:$E,A72))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L72" s="2">
+        <v>363058940.41379607</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>24</v>
+      </c>
+      <c r="J73">
+        <f>INDEX($G:$G,A73)</f>
+        <v>375827441</v>
+      </c>
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>24</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="J74">
+        <f>INDEX($G:G,A74)</f>
+        <v>0</v>
+      </c>
+      <c r="L74" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="M74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>25</v>
+      </c>
+      <c r="C75">
+        <v>25</v>
+      </c>
+      <c r="D75" t="s">
+        <v>64</v>
+      </c>
+      <c r="E75">
+        <v>0.98158623830724301</v>
+      </c>
+      <c r="G75" s="2">
+        <v>322511</v>
+      </c>
+      <c r="J75" t="e">
+        <f>INDEX($G:$G,A75)*(INDEX($E:$E,A75))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L75" s="2">
+        <v>316572.35930270725</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>25</v>
+      </c>
+      <c r="J76">
+        <f>INDEX($G:$G,A76)</f>
+        <v>322511</v>
+      </c>
+      <c r="L76" s="2"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>25</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="H77">
+        <v>1</v>
+      </c>
+      <c r="J77">
+        <f>INDEX($G:G,A77)</f>
+        <v>0</v>
+      </c>
+      <c r="L77" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="M77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>26</v>
+      </c>
+      <c r="C78">
+        <v>26</v>
+      </c>
+      <c r="D78" t="s">
+        <v>78</v>
+      </c>
+      <c r="E78">
+        <v>0.98989450947836999</v>
+      </c>
+      <c r="G78" s="2">
+        <v>7852929</v>
+      </c>
+      <c r="J78" t="e">
+        <f>INDEX($G:$G,A78)*(INDEX($E:$E,A78))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L78" s="2">
+        <v>7773571.3004234666</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>26</v>
+      </c>
+      <c r="J79">
+        <f>INDEX($G:$G,A79)</f>
+        <v>7852929</v>
+      </c>
+      <c r="L79" s="2"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>26</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="H80">
+        <v>1</v>
+      </c>
+      <c r="J80">
+        <f>INDEX($G:G,A80)</f>
+        <v>0</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="M80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>27</v>
+      </c>
+      <c r="C81">
+        <v>27</v>
+      </c>
+      <c r="D81" t="s">
+        <v>82</v>
+      </c>
+      <c r="E81">
+        <v>0.97743295410891196</v>
+      </c>
+      <c r="G81" s="2">
+        <v>12528066</v>
+      </c>
+      <c r="J81" t="e">
+        <f>INDEX($G:$G,A81)*(INDEX($E:$E,A81))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L81" s="2">
+        <v>12245344.55965142</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>27</v>
+      </c>
+      <c r="J82">
+        <f>INDEX($G:$G,A82)</f>
+        <v>12528066</v>
+      </c>
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>27</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <f>INDEX($G:G,A83)</f>
+        <v>0</v>
+      </c>
+      <c r="L83" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="M83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>28</v>
+      </c>
+      <c r="C84">
+        <v>28</v>
+      </c>
+      <c r="D84" t="s">
+        <v>32</v>
+      </c>
+      <c r="E84">
+        <v>0.98120167813382198</v>
+      </c>
+      <c r="G84" s="2">
+        <v>129703</v>
+      </c>
+      <c r="J84" t="e">
+        <f>INDEX($G:$G,A84)*(INDEX($E:$E,A84))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L84" s="2">
+        <v>127264.80125899111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>28</v>
+      </c>
+      <c r="J85">
+        <f>INDEX($G:$G,A85)</f>
+        <v>129703</v>
+      </c>
+      <c r="L85" s="2"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>28</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="H86">
+        <v>1</v>
+      </c>
+      <c r="J86">
+        <f>INDEX($G:G,A86)</f>
+        <v>0</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="M86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>29</v>
+      </c>
+      <c r="C87">
+        <v>29</v>
+      </c>
+      <c r="D87" t="s">
+        <v>88</v>
+      </c>
+      <c r="E87">
+        <v>0.98177814443945</v>
+      </c>
+      <c r="G87" s="2">
+        <v>2855160</v>
+      </c>
+      <c r="J87" t="e">
+        <f>INDEX($G:$G,A87)*(INDEX($E:$E,A87))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L87" s="2">
+        <v>2803133.6868777401</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>29</v>
+      </c>
+      <c r="J88">
+        <f>INDEX($G:$G,A88)</f>
+        <v>2855160</v>
+      </c>
+      <c r="L88" s="2"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>29</v>
+      </c>
+      <c r="G89" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="H89">
+        <v>1</v>
+      </c>
+      <c r="J89">
+        <f>INDEX($G:G,A89)</f>
+        <v>0</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="M89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>30</v>
+      </c>
+      <c r="C90">
+        <v>30</v>
+      </c>
+      <c r="D90" t="s">
+        <v>108</v>
+      </c>
+      <c r="E90">
+        <v>0.981979926302049</v>
+      </c>
+      <c r="G90" s="2">
+        <v>18518</v>
+      </c>
+      <c r="J90" t="e">
+        <f>INDEX($G:$G,A90)*(INDEX($E:$E,A90))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L90" s="2">
+        <v>18184.304275261344</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>30</v>
+      </c>
+      <c r="J91">
+        <f>INDEX($G:$G,A91)</f>
+        <v>18518</v>
+      </c>
+      <c r="L91" s="2"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>30</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="H92">
+        <v>1</v>
+      </c>
+      <c r="J92">
+        <f>INDEX($G:G,A92)</f>
+        <v>0</v>
+      </c>
+      <c r="L92" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="M92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>31</v>
+      </c>
+      <c r="C93">
+        <v>31</v>
+      </c>
+      <c r="D93" t="s">
+        <v>8</v>
+      </c>
+      <c r="E93">
+        <v>0.98620174158078799</v>
+      </c>
+      <c r="G93" s="2">
+        <v>58754062</v>
+      </c>
+      <c r="J93" t="e">
+        <f>INDEX($G:$G,A93)*(INDEX($E:$E,A93))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L93" s="2">
+        <v>57943358.269345596</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>31</v>
+      </c>
+      <c r="J94">
+        <f>INDEX($G:$G,A94)</f>
+        <v>58754062</v>
+      </c>
+      <c r="L94" s="2"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>31</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="H95">
+        <v>1</v>
+      </c>
+      <c r="J95">
+        <f>INDEX($G:G,A95)</f>
+        <v>0</v>
+      </c>
+      <c r="L95" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="M95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>32</v>
+      </c>
+      <c r="C96">
+        <v>32</v>
+      </c>
+      <c r="D96" t="s">
+        <v>62</v>
+      </c>
+      <c r="E96">
+        <v>0.98618575596674996</v>
+      </c>
+      <c r="G96" s="2">
+        <v>9568147</v>
+      </c>
+      <c r="J96" t="e">
+        <f>INDEX($G:$G,A96)*(INDEX($E:$E,A96))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L96" s="2">
+        <v>9435970.2823959906</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>32</v>
+      </c>
+      <c r="J97">
+        <f>INDEX($G:$G,A97)</f>
+        <v>9568147</v>
+      </c>
+      <c r="L97" s="2"/>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>32</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="J98">
+        <f>INDEX($G:G,A98)</f>
+        <v>0</v>
+      </c>
+      <c r="L98" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="M98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>33</v>
+      </c>
+      <c r="C99">
+        <v>33</v>
+      </c>
+      <c r="D99" t="s">
+        <v>24</v>
+      </c>
+      <c r="E99">
+        <v>0.983873842655416</v>
+      </c>
+      <c r="G99">
+        <v>515</v>
+      </c>
+      <c r="J99" t="e">
+        <f>INDEX($G:$G,A99)*(INDEX($E:$E,A99))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L99" s="2">
+        <v>506.69502896753926</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>33</v>
+      </c>
+      <c r="J100">
+        <f>INDEX($G:$G,A100)</f>
+        <v>515</v>
+      </c>
+      <c r="L100" s="2"/>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>33</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="H101">
+        <v>1</v>
+      </c>
+      <c r="J101">
+        <f>INDEX($G:G,A101)</f>
+        <v>0</v>
+      </c>
+      <c r="L101" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="M101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>34</v>
+      </c>
+      <c r="C102">
+        <v>34</v>
+      </c>
+      <c r="D102" t="s">
+        <v>40</v>
+      </c>
+      <c r="E102">
+        <v>0.977253000905142</v>
+      </c>
+      <c r="G102" s="2">
+        <v>80012</v>
+      </c>
+      <c r="J102" t="e">
+        <f>INDEX($G:$G,A102)*(INDEX($E:$E,A102))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L102" s="2">
+        <v>78191.967108422221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>34</v>
+      </c>
+      <c r="J103">
+        <f>INDEX($G:$G,A103)</f>
+        <v>80012</v>
+      </c>
+      <c r="L103" s="2"/>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>34</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="H104">
+        <v>1</v>
+      </c>
+      <c r="J104">
+        <f>INDEX($G:G,A104)</f>
+        <v>0</v>
+      </c>
+      <c r="L104" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="M104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>35</v>
+      </c>
+      <c r="C105">
+        <v>35</v>
+      </c>
+      <c r="D105" t="s">
+        <v>102</v>
+      </c>
+      <c r="E105">
+        <v>0.97763416898382804</v>
+      </c>
+      <c r="G105" s="2">
+        <v>113160</v>
+      </c>
+      <c r="J105" t="e">
+        <f>INDEX($G:$G,A105)*(INDEX($E:$E,A105))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L105" s="2">
+        <v>110629.08256220998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>35</v>
+      </c>
+      <c r="J106">
+        <f>INDEX($G:$G,A106)</f>
+        <v>113160</v>
+      </c>
+      <c r="L106" s="2"/>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>35</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="H107">
+        <v>1</v>
+      </c>
+      <c r="J107">
+        <f>INDEX($G:G,A107)</f>
+        <v>0</v>
+      </c>
+      <c r="L107" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="M107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>36</v>
+      </c>
+      <c r="C108">
+        <v>36</v>
+      </c>
+      <c r="D108" t="s">
+        <v>106</v>
+      </c>
+      <c r="E108">
+        <v>0.97765261116189095</v>
+      </c>
+      <c r="G108" s="2">
+        <v>72455</v>
+      </c>
+      <c r="J108" t="e">
+        <f>INDEX($G:$G,A108)*(INDEX($E:$E,A108))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L108" s="2">
+        <v>70835.819941734808</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>36</v>
+      </c>
+      <c r="J109">
+        <f>INDEX($G:$G,A109)</f>
+        <v>72455</v>
+      </c>
+      <c r="L109" s="2"/>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>36</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="H110">
+        <v>1</v>
+      </c>
+      <c r="J110">
+        <f>INDEX($G:G,A110)</f>
+        <v>0</v>
+      </c>
+      <c r="L110" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="M110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>37</v>
+      </c>
+      <c r="C111">
+        <v>37</v>
+      </c>
+      <c r="D111" t="s">
+        <v>122</v>
+      </c>
+      <c r="E111">
+        <v>0.98992729736486695</v>
+      </c>
+      <c r="G111" s="2">
+        <v>998417</v>
+      </c>
+      <c r="J111" t="e">
+        <f>INDEX($G:$G,A111)*(INDEX($E:$E,A111))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L111" s="2">
+        <v>988360.24245313834</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A112">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>37</v>
+      </c>
+      <c r="J112">
+        <f>INDEX($G:$G,A112)</f>
+        <v>998417</v>
+      </c>
+      <c r="L112" s="2"/>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>37</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="H113">
+        <v>1</v>
+      </c>
+      <c r="J113">
+        <f>INDEX($G:G,A113)</f>
+        <v>0</v>
+      </c>
+      <c r="L113" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="M113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>38</v>
+      </c>
+      <c r="C114">
+        <v>38</v>
+      </c>
+      <c r="D114" t="s">
+        <v>26</v>
+      </c>
+      <c r="E114">
+        <v>0.99010920504213995</v>
+      </c>
+      <c r="G114" s="2">
+        <v>13254</v>
+      </c>
+      <c r="J114" t="e">
+        <f>INDEX($G:$G,A114)*(INDEX($E:$E,A114))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L114" s="2">
+        <v>13122.907403628524</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>38</v>
+      </c>
+      <c r="J115">
+        <f>INDEX($G:$G,A115)</f>
+        <v>13254</v>
+      </c>
+      <c r="L115" s="2"/>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>38</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="H116">
+        <v>1</v>
+      </c>
+      <c r="J116">
+        <f>INDEX($G:G,A116)</f>
+        <v>0</v>
+      </c>
+      <c r="L116" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="M116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>39</v>
+      </c>
+      <c r="C117">
+        <v>39</v>
+      </c>
+      <c r="D117" t="s">
+        <v>56</v>
+      </c>
+      <c r="E117">
+        <v>0.98993762881686898</v>
+      </c>
+      <c r="G117" s="2">
+        <v>177873933</v>
+      </c>
+      <c r="J117" t="e">
+        <f>INDEX($G:$G,A117)*(INDEX($E:$E,A117))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L117" s="2">
+        <v>176084099.46235061</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>39</v>
+      </c>
+      <c r="J118">
+        <f>INDEX($G:$G,A118)</f>
+        <v>177873933</v>
+      </c>
+      <c r="L118" s="2"/>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>39</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+      <c r="J119">
+        <f>INDEX($G:G,A119)</f>
+        <v>0</v>
+      </c>
+      <c r="L119" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="M119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>40</v>
+      </c>
+      <c r="C120">
+        <v>40</v>
+      </c>
+      <c r="D120" t="s">
+        <v>44</v>
+      </c>
+      <c r="E120">
+        <v>0.98130314557887499</v>
+      </c>
+      <c r="G120" s="2">
+        <v>104562460</v>
+      </c>
+      <c r="J120" t="e">
+        <f>INDEX($G:$G,A120)*(INDEX($E:$E,A120))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L120" s="2">
+        <v>102607470.90746529</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>40</v>
+      </c>
+      <c r="J121">
+        <f>INDEX($G:$G,A121)</f>
+        <v>104562460</v>
+      </c>
+      <c r="L121" s="2"/>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>40</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="H122">
+        <v>1</v>
+      </c>
+      <c r="J122">
+        <f>INDEX($G:G,A122)</f>
+        <v>0</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="M122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>41</v>
+      </c>
+      <c r="C123">
+        <v>41</v>
+      </c>
+      <c r="D123" t="s">
+        <v>124</v>
+      </c>
+      <c r="E123">
+        <v>1.00224396572352</v>
+      </c>
+      <c r="G123" s="2">
+        <v>210750273</v>
+      </c>
+      <c r="J123" t="e">
+        <f>INDEX($G:$G,A123)*(INDEX($E:$E,A123))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L123" s="2">
+        <v>211223189.38883448</v>
+      </c>
+    </row>
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>41</v>
+      </c>
+      <c r="J124">
+        <f>INDEX($G:$G,A124)</f>
+        <v>210750273</v>
+      </c>
+      <c r="L124" s="2"/>
+    </row>
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>41</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="H125">
+        <v>1</v>
+      </c>
+      <c r="J125">
+        <f>INDEX($G:G,A125)</f>
+        <v>0</v>
+      </c>
+      <c r="L125" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="M125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>42</v>
+      </c>
+      <c r="C126">
+        <v>42</v>
+      </c>
+      <c r="D126" t="s">
+        <v>100</v>
+      </c>
+      <c r="E126">
+        <v>1.2625994430592999</v>
+      </c>
+      <c r="G126" s="2">
+        <v>24396481</v>
+      </c>
+      <c r="J126" t="e">
+        <f>INDEX($G:$G,A126)*(INDEX($E:$E,A126))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L126" s="2">
+        <v>30802983.323206794</v>
+      </c>
+    </row>
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>42</v>
+      </c>
+      <c r="J127">
+        <f>INDEX($G:$G,A127)</f>
+        <v>24396481</v>
+      </c>
+      <c r="L127" s="2"/>
+    </row>
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>42</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="H128">
+        <v>1</v>
+      </c>
+      <c r="J128">
+        <f>INDEX($G:G,A128)</f>
+        <v>0</v>
+      </c>
+      <c r="L128" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="M128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>43</v>
+      </c>
+      <c r="C129">
+        <v>43</v>
+      </c>
+      <c r="D129" t="s">
+        <v>98</v>
+      </c>
+      <c r="E129">
+        <v>0.99472956131107804</v>
+      </c>
+      <c r="G129" s="2">
+        <v>221366</v>
+      </c>
+      <c r="J129" t="e">
+        <f>INDEX($G:$G,A129)*(INDEX($E:$E,A129))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L129" s="2">
+        <v>220199.3040691881</v>
+      </c>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>43</v>
+      </c>
+      <c r="J130">
+        <f>INDEX($G:$G,A130)</f>
+        <v>221366</v>
+      </c>
+      <c r="L130" s="2"/>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>43</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="H131">
+        <v>1</v>
+      </c>
+      <c r="J131">
+        <f>INDEX($G:G,A131)</f>
+        <v>0</v>
+      </c>
+      <c r="L131" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="M131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>44</v>
+      </c>
+      <c r="C132">
+        <v>44</v>
+      </c>
+      <c r="D132" t="s">
+        <v>86</v>
+      </c>
+      <c r="E132">
+        <v>0.99482226936644302</v>
+      </c>
+      <c r="G132" s="2">
+        <v>10432</v>
+      </c>
+      <c r="J132" t="e">
+        <f>INDEX($G:$G,A132)*(INDEX($E:$E,A132))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L132" s="2">
+        <v>10377.985914030734</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>44</v>
+      </c>
+      <c r="J133">
+        <f>INDEX($G:$G,A133)</f>
+        <v>10432</v>
+      </c>
+      <c r="L133" s="2"/>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>44</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="H134">
+        <v>1</v>
+      </c>
+      <c r="J134">
+        <f>INDEX($G:G,A134)</f>
+        <v>0</v>
+      </c>
+      <c r="L134" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="M134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>45</v>
+      </c>
+      <c r="C135">
+        <v>45</v>
+      </c>
+      <c r="D135" t="s">
+        <v>68</v>
+      </c>
+      <c r="E135">
+        <v>0.99417365434823801</v>
+      </c>
+      <c r="G135" s="2">
+        <v>296</v>
+      </c>
+      <c r="J135" t="e">
+        <f>INDEX($G:$G,A135)*(INDEX($E:$E,A135))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L135" s="2">
+        <v>294.27540168707844</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>45</v>
+      </c>
+      <c r="J136">
+        <f>INDEX($G:$G,A136)</f>
+        <v>296</v>
+      </c>
+      <c r="L136" s="2"/>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>45</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="H137">
+        <v>1</v>
+      </c>
+      <c r="J137">
+        <f>INDEX($G:G,A137)</f>
+        <v>0</v>
+      </c>
+      <c r="L137" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="M137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>46</v>
+      </c>
+      <c r="C138">
+        <v>46</v>
+      </c>
+      <c r="D138" t="s">
+        <v>36</v>
+      </c>
+      <c r="E138">
+        <v>0.99104885024245204</v>
+      </c>
+      <c r="G138" s="2">
+        <v>2151</v>
+      </c>
+      <c r="J138" t="e">
+        <f>INDEX($G:$G,A138)*(INDEX($E:$E,A138))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L138" s="2">
+        <v>2131.7460768715146</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>46</v>
+      </c>
+      <c r="J139">
+        <f>INDEX($G:$G,A139)</f>
+        <v>2151</v>
+      </c>
+      <c r="L139" s="2"/>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>139</v>
+      </c>
+      <c r="B140">
+        <v>46</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="H140">
+        <v>1</v>
+      </c>
+      <c r="J140">
+        <f>INDEX($G:G,A140)</f>
+        <v>0</v>
+      </c>
+      <c r="L140" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="M140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>140</v>
+      </c>
+      <c r="B141">
+        <v>47</v>
+      </c>
+      <c r="C141">
+        <v>47</v>
+      </c>
+      <c r="D141" t="s">
+        <v>80</v>
+      </c>
+      <c r="E141">
+        <v>0.99142615553283597</v>
+      </c>
+      <c r="G141" s="2">
+        <v>686</v>
+      </c>
+      <c r="J141" t="e">
+        <f>INDEX($G:$G,A141)*(INDEX($E:$E,A141))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L141" s="2">
+        <v>680.11834269552548</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>141</v>
+      </c>
+      <c r="B142">
+        <v>47</v>
+      </c>
+      <c r="J142">
+        <f>INDEX($G:$G,A142)</f>
+        <v>686</v>
+      </c>
+      <c r="L142" s="2"/>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>142</v>
+      </c>
+      <c r="B143">
+        <v>47</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <f>INDEX($G:G,A143)</f>
+        <v>0</v>
+      </c>
+      <c r="L143" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="M143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>143</v>
+      </c>
+      <c r="B144">
+        <v>48</v>
+      </c>
+      <c r="C144">
+        <v>48</v>
+      </c>
+      <c r="D144" t="s">
+        <v>72</v>
+      </c>
+      <c r="E144">
+        <v>0.99032845029036998</v>
+      </c>
+      <c r="G144" s="2">
+        <v>499</v>
+      </c>
+      <c r="J144" t="e">
+        <f>INDEX($G:$G,A144)*(INDEX($E:$E,A144))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L144" s="2">
+        <v>494.17389669489461</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>144</v>
+      </c>
+      <c r="B145">
+        <v>48</v>
+      </c>
+      <c r="J145">
+        <f>INDEX($G:$G,A145)</f>
+        <v>499</v>
+      </c>
+      <c r="L145" s="2"/>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>145</v>
+      </c>
+      <c r="B146">
+        <v>48</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H146">
+        <v>1</v>
+      </c>
+      <c r="J146">
+        <f>INDEX($G:G,A146)</f>
+        <v>0</v>
+      </c>
+      <c r="L146" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="M146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>146</v>
+      </c>
+      <c r="B147">
+        <v>49</v>
+      </c>
+      <c r="C147">
+        <v>49</v>
+      </c>
+      <c r="D147" t="s">
+        <v>118</v>
+      </c>
+      <c r="E147">
+        <v>1.5544005589154499</v>
+      </c>
+      <c r="G147" s="2">
+        <v>5018603</v>
+      </c>
+      <c r="J147" t="e">
+        <f>INDEX($G:$G,A147)*(INDEX($E:$E,A147))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L147" s="2">
+        <v>7800919.3081747536</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>147</v>
+      </c>
+      <c r="B148">
+        <v>49</v>
+      </c>
+      <c r="J148">
+        <f>INDEX($G:$G,A148)</f>
+        <v>5018603</v>
+      </c>
+      <c r="L148" s="2"/>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>148</v>
+      </c>
+      <c r="B149">
+        <v>49</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="H149">
+        <v>1</v>
+      </c>
+      <c r="J149">
+        <f>INDEX($G:G,A149)</f>
+        <v>0</v>
+      </c>
+      <c r="L149" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="M149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>149</v>
+      </c>
+      <c r="B150">
+        <v>50</v>
+      </c>
+      <c r="C150">
+        <v>50</v>
+      </c>
+      <c r="D150" t="s">
+        <v>48</v>
+      </c>
+      <c r="E150">
+        <v>0.99390763097371004</v>
+      </c>
+      <c r="G150" s="2">
+        <v>7042431</v>
+      </c>
+      <c r="J150" t="e">
+        <f>INDEX($G:$G,A150)*(INDEX($E:$E,A150))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L150" s="2">
+        <v>6999525.9115058156</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>150</v>
+      </c>
+      <c r="B151">
+        <v>50</v>
+      </c>
+      <c r="J151">
+        <f>INDEX($G:$G,A151)</f>
+        <v>7042431</v>
+      </c>
+      <c r="L151" s="2"/>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>151</v>
+      </c>
+      <c r="B152">
+        <v>50</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+      <c r="J152">
+        <f>INDEX($G:G,A152)</f>
+        <v>0</v>
+      </c>
+      <c r="L152" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="M152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>152</v>
+      </c>
+      <c r="B153">
+        <v>51</v>
+      </c>
+      <c r="C153">
+        <v>51</v>
+      </c>
+      <c r="D153" t="s">
+        <v>60</v>
+      </c>
+      <c r="E153">
+        <v>0.99315190485392801</v>
+      </c>
+      <c r="G153" s="2">
+        <v>1465244</v>
+      </c>
+      <c r="J153" t="e">
+        <f>INDEX($G:$G,A153)*(INDEX($E:$E,A153))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L153" s="2">
+        <v>1455209.8696757888</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A154">
+        <v>153</v>
+      </c>
+      <c r="B154">
+        <v>51</v>
+      </c>
+      <c r="J154">
+        <f>INDEX($G:$G,A154)</f>
+        <v>1465244</v>
+      </c>
+      <c r="L154" s="2"/>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A155">
+        <v>154</v>
+      </c>
+      <c r="B155">
+        <v>51</v>
+      </c>
+      <c r="G155" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="H155">
+        <v>1</v>
+      </c>
+      <c r="J155">
+        <f>INDEX($G:G,A155)</f>
+        <v>0</v>
+      </c>
+      <c r="L155" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="M155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A156">
+        <v>155</v>
+      </c>
+      <c r="B156">
+        <v>52</v>
+      </c>
+      <c r="C156">
+        <v>52</v>
+      </c>
+      <c r="D156" t="s">
+        <v>90</v>
+      </c>
+      <c r="E156">
+        <v>2.4151325594945399</v>
+      </c>
+      <c r="G156" s="2">
+        <v>1152057</v>
+      </c>
+      <c r="J156" t="e">
+        <f>INDEX($G:$G,A156)*(INDEX($E:$E,A156))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L156" s="2">
+        <v>2782370.371093601</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A157">
+        <v>156</v>
+      </c>
+      <c r="B157">
+        <v>52</v>
+      </c>
+      <c r="J157">
+        <f>INDEX($G:$G,A157)</f>
+        <v>1152057</v>
+      </c>
+      <c r="L157" s="2"/>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A158">
+        <v>157</v>
+      </c>
+      <c r="B158">
+        <v>52</v>
+      </c>
+      <c r="G158" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="H158">
+        <v>1</v>
+      </c>
+      <c r="J158">
+        <f>INDEX($G:G,A158)</f>
+        <v>0</v>
+      </c>
+      <c r="L158" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="M158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A159">
+        <v>158</v>
+      </c>
+      <c r="B159">
+        <v>53</v>
+      </c>
+      <c r="C159">
+        <v>53</v>
+      </c>
+      <c r="D159" t="s">
+        <v>76</v>
+      </c>
+      <c r="E159">
+        <v>1.33527733145297</v>
+      </c>
+      <c r="G159" s="2">
+        <v>19389</v>
+      </c>
+      <c r="J159" t="e">
+        <f>INDEX($G:$G,A159)*(INDEX($E:$E,A159))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L159" s="2">
+        <v>25889.692179541635</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>159</v>
+      </c>
+      <c r="B160">
+        <v>53</v>
+      </c>
+      <c r="J160">
+        <f>INDEX($G:$G,A160)</f>
+        <v>19389</v>
+      </c>
+      <c r="L160" s="2"/>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161">
+        <v>53</v>
+      </c>
+      <c r="G161" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="H161">
+        <v>1</v>
+      </c>
+      <c r="J161">
+        <f>INDEX($G:G,A161)</f>
+        <v>0</v>
+      </c>
+      <c r="L161" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="M161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162">
+        <v>54</v>
+      </c>
+      <c r="C162">
+        <v>54</v>
+      </c>
+      <c r="D162" t="s">
+        <v>52</v>
+      </c>
+      <c r="E162">
+        <v>0.99831748425879197</v>
+      </c>
+      <c r="G162" s="2">
+        <v>197</v>
+      </c>
+      <c r="J162" t="e">
+        <f>INDEX($G:$G,A162)*(INDEX($E:$E,A162))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L162" s="2">
+        <v>196.66854439898202</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163">
+        <v>54</v>
+      </c>
+      <c r="J163">
+        <f>INDEX($G:$G,A163)</f>
+        <v>197</v>
+      </c>
+      <c r="L163" s="2"/>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164">
+        <v>54</v>
+      </c>
+      <c r="G164" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="H164">
+        <v>1</v>
+      </c>
+      <c r="J164">
+        <f>INDEX($G:G,A164)</f>
+        <v>0</v>
+      </c>
+      <c r="L164" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="M164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165">
+        <v>55</v>
+      </c>
+      <c r="C165">
+        <v>55</v>
+      </c>
+      <c r="D165" t="s">
+        <v>84</v>
+      </c>
+      <c r="E165">
+        <v>1.00078452001425</v>
+      </c>
+      <c r="G165" s="2">
+        <v>11</v>
+      </c>
+      <c r="J165" t="e">
+        <f>INDEX($G:$G,A165)*(INDEX($E:$E,A165))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L165" s="2">
+        <v>11.008629720156749</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166">
+        <v>55</v>
+      </c>
+      <c r="J166">
+        <f>INDEX($G:$G,A166)</f>
+        <v>11</v>
+      </c>
+      <c r="L166" s="2"/>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167">
+        <v>55</v>
+      </c>
+      <c r="G167" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="H167">
+        <v>1</v>
+      </c>
+      <c r="J167">
+        <f>INDEX($G:G,A167)</f>
+        <v>0</v>
+      </c>
+      <c r="L167" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="M167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168">
+        <v>56</v>
+      </c>
+      <c r="C168">
+        <v>56</v>
+      </c>
+      <c r="D168" t="s">
+        <v>28</v>
+      </c>
+      <c r="E168">
+        <v>0.99926374319143496</v>
+      </c>
+      <c r="G168" s="2">
+        <v>54</v>
+      </c>
+      <c r="J168" t="e">
+        <f>INDEX($G:$G,A168)*(INDEX($E:$E,A168))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L168" s="2">
+        <v>53.960242132337491</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169">
+        <v>56</v>
+      </c>
+      <c r="J169">
+        <f>INDEX($G:$G,A169)</f>
+        <v>54</v>
+      </c>
+      <c r="L169" s="2"/>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170">
+        <v>56</v>
+      </c>
+      <c r="G170" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="H170">
+        <v>1</v>
+      </c>
+      <c r="J170">
+        <f>INDEX($G:G,A170)</f>
+        <v>0</v>
+      </c>
+      <c r="L170" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="M170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171">
+        <v>57</v>
+      </c>
+      <c r="C171">
+        <v>57</v>
+      </c>
+      <c r="D171" t="s">
+        <v>96</v>
+      </c>
+      <c r="E171">
+        <v>1.00112294550547</v>
+      </c>
+      <c r="G171" s="2">
+        <v>2110</v>
+      </c>
+      <c r="J171" t="e">
+        <f>INDEX($G:$G,A171)*(INDEX($E:$E,A171))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L171" s="2">
+        <v>2112.3694150165416</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172">
+        <v>57</v>
+      </c>
+      <c r="J172">
+        <f>INDEX($G:$G,A172)</f>
+        <v>2110</v>
+      </c>
+      <c r="L172" s="2"/>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173">
+        <v>57</v>
+      </c>
+      <c r="G173" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="H173">
+        <v>1</v>
+      </c>
+      <c r="J173">
+        <f>INDEX($G:G,A173)</f>
+        <v>0</v>
+      </c>
+      <c r="L173" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="M173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174">
+        <v>58</v>
+      </c>
+      <c r="C174">
+        <v>58</v>
+      </c>
+      <c r="D174" t="s">
+        <v>110</v>
+      </c>
+      <c r="E174">
+        <v>0.99451376832671601</v>
+      </c>
+      <c r="G174" s="2">
+        <v>24</v>
+      </c>
+      <c r="J174" t="e">
+        <f>INDEX($G:$G,A174)*(INDEX($E:$E,A174))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L174" s="2">
+        <v>23.868330439841184</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175">
+        <v>58</v>
+      </c>
+      <c r="J175">
+        <f>INDEX($G:$G,A175)</f>
+        <v>24</v>
+      </c>
+      <c r="L175" s="2"/>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176">
+        <v>58</v>
+      </c>
+      <c r="G176" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="H176">
+        <v>1</v>
+      </c>
+      <c r="J176">
+        <f>INDEX($G:G,A176)</f>
+        <v>0</v>
+      </c>
+      <c r="L176" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="M176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177">
+        <v>59</v>
+      </c>
+      <c r="C177">
+        <v>59</v>
+      </c>
+      <c r="D177" t="s">
+        <v>46</v>
+      </c>
+      <c r="E177">
+        <v>0.98926395449688098</v>
+      </c>
+      <c r="G177" s="2">
+        <v>532555</v>
+      </c>
+      <c r="J177" t="e">
+        <f>INDEX($G:$G,A177)*(INDEX($E:$E,A177))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L177" s="2">
+        <v>526837.46528708644</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178">
+        <v>59</v>
+      </c>
+      <c r="G178" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J178">
+        <f>INDEX($G:$G,A178)</f>
+        <v>532555</v>
+      </c>
+      <c r="L178" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A1:M178">
+    <sortCondition ref="A1:A178"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K93"/>
   <sheetViews>

</xml_diff>